<commit_message>
Final draft of report
</commit_message>
<xml_diff>
--- a/Submissions/4_Pandas/HeroesOfPymoli/PyMoliTables.xlsx
+++ b/Submissions/4_Pandas/HeroesOfPymoli/PyMoliTables.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slapp\Desktop\SMU_Homework\Submissions\4_Pandas\HeroesOfPymoli\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067EB973-FBBB-4AB5-AE79-D4E81FF05A95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73" yWindow="7107" windowWidth="20187" windowHeight="12920" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="purchsum" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
     <sheet name="top_seller" sheetId="7" r:id="rId7"/>
     <sheet name="top_earner" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -383,8 +377,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,18 +395,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -442,23 +430,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,14 +441,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -520,7 +487,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -552,27 +519,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -604,24 +553,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -797,14 +728,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -818,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -841,14 +772,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -859,7 +790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -873,7 +804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -887,7 +818,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -901,7 +832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -921,14 +852,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -948,7 +879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -971,7 +902,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -994,7 +925,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1023,14 +954,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1041,7 +972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1055,7 +986,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1069,7 +1000,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1083,7 +1014,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1097,7 +1028,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1111,7 +1042,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1125,7 +1056,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1139,7 +1070,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1159,208 +1090,214 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="B1:G9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2">
         <v>23</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3">
         <v>28</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4">
         <v>136</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5">
         <v>365</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6">
         <v>101</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7">
         <v>73</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8">
         <v>41</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9">
         <v>13</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1370,22 +1307,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>78</v>
       </c>
@@ -1399,8 +1328,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
         <v>79</v>
       </c>
@@ -1414,8 +1345,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
         <v>80</v>
       </c>
@@ -1429,8 +1362,10 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
         <v>81</v>
       </c>
@@ -1444,8 +1379,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
       <c r="B5" t="s">
         <v>82</v>
       </c>
@@ -1459,8 +1396,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
       <c r="B6" t="s">
         <v>83</v>
       </c>
@@ -1480,14 +1419,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>95</v>
       </c>
@@ -1504,7 +1443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>92</v>
       </c>
@@ -1521,7 +1460,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>178</v>
       </c>
@@ -1538,7 +1477,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>145</v>
       </c>
@@ -1555,7 +1494,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>132</v>
       </c>
@@ -1572,7 +1511,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>108</v>
       </c>
@@ -1595,14 +1534,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>95</v>
       </c>
@@ -1619,7 +1558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>92</v>
       </c>
@@ -1636,7 +1575,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>178</v>
       </c>
@@ -1653,7 +1592,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>82</v>
       </c>
@@ -1670,7 +1609,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>145</v>
       </c>
@@ -1687,7 +1626,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>103</v>
       </c>

</xml_diff>